<commit_message>
updated browser to chrome
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harjeet Singh\Documents\GitHub\sg-altonomy-qa\src\test\resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A415E0C-B936-405F-9CA8-F462F1595BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DC8064-0197-427C-9B3F-70D161EA5414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -209,7 +209,7 @@
     <t>Altonomy</t>
   </si>
   <si>
-    <t>FIREFOX</t>
+    <t>Chrome</t>
   </si>
 </sst>
 </file>
@@ -677,7 +677,7 @@
   <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
Fixed null pointer exception in ExcelDataUtil.java
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arjun Diwan\Documents\GitHub\sg-altonomy-qa\src\test\resources\ExcelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harjeet Singh\Documents\GitHub\sg-altonomy-qa\src\test\resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806EE156-32A3-4D2B-AE5F-2455D2FB217F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3A769B-EA95-40AD-B902-CCF99399D4A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="61">
   <si>
     <t>Tx-Automate: SETTINGS</t>
   </si>
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1002,7 +1002,9 @@
       <c r="A30" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="10"/>
+      <c r="B30" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -1011,7 +1013,9 @@
       <c r="A31" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="10"/>
+      <c r="B31" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="10"/>
@@ -1019,6 +1023,9 @@
     <row r="32" spans="1:7" ht="15.5">
       <c r="A32" s="11" t="s">
         <v>41</v>
+      </c>
+      <c r="B32" t="s">
+        <v>52</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -1029,7 +1036,9 @@
       <c r="A33" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="3"/>
+      <c r="B33" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>

</xml_diff>